<commit_message>
add phenotypes and covariates for cohort 9
</commit_message>
<xml_diff>
--- a/CREATE/cocaine_c01_boxes_toqc.xlsx
+++ b/CREATE/cocaine_c01_boxes_toqc.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t xml:space="preserve">cohort</t>
   </si>
@@ -59,97 +59,121 @@
     <t xml:space="preserve">F1</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">1110-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-1</t>
   </si>
   <si>
     <t xml:space="preserve">F2</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">1110-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-2</t>
   </si>
   <si>
     <t xml:space="preserve">F3</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
+    <t xml:space="preserve">1110-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-3</t>
   </si>
   <si>
     <t xml:space="preserve">F4</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
+    <t xml:space="preserve">1110-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-4</t>
   </si>
   <si>
     <t xml:space="preserve">F5</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
+    <t xml:space="preserve">1110-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-5</t>
   </si>
   <si>
     <t xml:space="preserve">F6</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
+    <t xml:space="preserve">1110-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-6</t>
   </si>
   <si>
     <t xml:space="preserve">F7</t>
   </si>
   <si>
-    <t xml:space="preserve">7</t>
+    <t xml:space="preserve">1110-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-7</t>
   </si>
   <si>
     <t xml:space="preserve">F8</t>
   </si>
   <si>
-    <t xml:space="preserve">8</t>
+    <t xml:space="preserve">1110-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-8</t>
   </si>
   <si>
     <t xml:space="preserve">F9</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">1110-9</t>
   </si>
   <si>
     <t xml:space="preserve">F10</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">1110-10</t>
   </si>
   <si>
     <t xml:space="preserve">F11</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
+    <t xml:space="preserve">1110-11</t>
   </si>
   <si>
     <t xml:space="preserve">F12</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">1110-12</t>
   </si>
   <si>
     <t xml:space="preserve">F13</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
+    <t xml:space="preserve">1110-13</t>
   </si>
   <si>
     <t xml:space="preserve">F14</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">1110-14</t>
   </si>
   <si>
     <t xml:space="preserve">F15</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">1110-15</t>
   </si>
   <si>
     <t xml:space="preserve">F16</t>
   </si>
   <si>
-    <t xml:space="preserve">16</t>
+    <t xml:space="preserve">1110-16</t>
   </si>
   <si>
     <t xml:space="preserve">F18</t>
@@ -200,12 +224,18 @@
     <t xml:space="preserve">K2-2</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-9</t>
+  </si>
+  <si>
     <t xml:space="preserve">M2</t>
   </si>
   <si>
     <t xml:space="preserve">K2-3</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">M3</t>
   </si>
   <si>
@@ -215,34 +245,52 @@
     <t xml:space="preserve">K2-4</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">M8</t>
   </si>
   <si>
     <t xml:space="preserve">K2-5</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-12</t>
+  </si>
+  <si>
     <t xml:space="preserve">M13</t>
   </si>
   <si>
     <t xml:space="preserve">K2-6</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-13</t>
+  </si>
+  <si>
     <t xml:space="preserve">M14</t>
   </si>
   <si>
     <t xml:space="preserve">K3-1</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-14</t>
+  </si>
+  <si>
     <t xml:space="preserve">M21</t>
   </si>
   <si>
     <t xml:space="preserve">K3-2</t>
   </si>
   <si>
+    <t xml:space="preserve">MED1110-15</t>
+  </si>
+  <si>
     <t xml:space="preserve">M22</t>
   </si>
   <si>
     <t xml:space="preserve">K3-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED1110-16</t>
   </si>
   <si>
     <t xml:space="preserve">M27</t>
@@ -712,13 +760,25 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
       <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
@@ -727,7 +787,7 @@
       </c>
       <c r="L2"/>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -735,24 +795,36 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
       <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -760,24 +832,36 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
       <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -785,24 +869,36 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
       <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L5"/>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -810,24 +906,36 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
       <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="L6"/>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -835,24 +943,36 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
       <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L7"/>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -860,24 +980,36 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
       <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -885,24 +1017,36 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
       <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L9"/>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -910,24 +1054,36 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
       <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -935,24 +1091,36 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L11"/>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -960,24 +1128,36 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
       <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -985,24 +1165,36 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
       <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -1010,24 +1202,36 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
       <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -1035,24 +1239,36 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
       <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
       <c r="J15" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="L15"/>
       <c r="M15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
@@ -1060,20 +1276,32 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
       <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="L16"/>
       <c r="M16"/>
@@ -1083,24 +1311,36 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
       <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
       <c r="J17" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="L17"/>
       <c r="M17" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
@@ -1108,40 +1348,40 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="J18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="L18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="M18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -1149,40 +1389,40 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="M19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -1190,40 +1430,40 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="K20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="L20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M20" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -1231,40 +1471,40 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="I21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="K21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L21" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
@@ -1272,40 +1512,40 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="L22" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M22" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
@@ -1313,40 +1553,40 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="I23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="L23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="M23" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
@@ -1354,40 +1594,40 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="I24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="K24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="M24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
@@ -1395,40 +1635,40 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="L25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="M25" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
@@ -1436,38 +1676,38 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G26"/>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="J26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="K26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="M26" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27">
@@ -1475,14 +1715,14 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -1496,40 +1736,40 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="J28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="L28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="M28" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -1537,40 +1777,40 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="I29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="J29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="K29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="L29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
@@ -1578,40 +1818,40 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="H30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="I30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="J30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="K30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="L30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="M30" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
@@ -1619,38 +1859,38 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="I31"/>
       <c r="J31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="K31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="L31" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="M31" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
@@ -1658,40 +1898,40 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="J32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="K32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="L32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="M32" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33">
@@ -1699,40 +1939,40 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="I33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="J33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="K33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="L33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="M33" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34">
@@ -1740,40 +1980,40 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="G34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="J34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="K34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="L34" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="M34" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35">
@@ -1781,40 +2021,40 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="H35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="I35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="J35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="K35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="L35" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="M35" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36">
@@ -1822,40 +2062,40 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="H36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="I36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="J36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="K36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="L36" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="M36" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37">
@@ -1863,40 +2103,40 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="I37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="J37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="K37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="L37" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="M37" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38">
@@ -1904,40 +2144,40 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="G38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="H38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="I38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="K38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="L38" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="M38" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39">
@@ -1945,40 +2185,40 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="G39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="H39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="J39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="K39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="L39" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="M39" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40">
@@ -1986,40 +2226,40 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" t="s">
+        <v>106</v>
+      </c>
+      <c r="J40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K40" t="s">
+        <v>106</v>
+      </c>
+      <c r="L40" t="s">
+        <v>106</v>
+      </c>
+      <c r="M40" t="s">
         <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" t="s">
-        <v>90</v>
-      </c>
-      <c r="G40" t="s">
-        <v>90</v>
-      </c>
-      <c r="H40" t="s">
-        <v>90</v>
-      </c>
-      <c r="I40" t="s">
-        <v>90</v>
-      </c>
-      <c r="J40" t="s">
-        <v>90</v>
-      </c>
-      <c r="K40" t="s">
-        <v>90</v>
-      </c>
-      <c r="L40" t="s">
-        <v>90</v>
-      </c>
-      <c r="M40" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="41">
@@ -2027,40 +2267,40 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" t="s">
+        <v>108</v>
+      </c>
+      <c r="J41" t="s">
+        <v>108</v>
+      </c>
+      <c r="K41" t="s">
+        <v>108</v>
+      </c>
+      <c r="L41" t="s">
+        <v>108</v>
+      </c>
+      <c r="M41" t="s">
         <v>92</v>
-      </c>
-      <c r="D41" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J41" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" t="s">
-        <v>92</v>
-      </c>
-      <c r="L41" t="s">
-        <v>92</v>
-      </c>
-      <c r="M41" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="42">
@@ -2068,40 +2308,40 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="F42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="G42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="H42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="I42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="L42" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="M42" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43">
@@ -2109,38 +2349,38 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="G43"/>
       <c r="H43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="I43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="J43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="L43" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="M43" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44">
@@ -2148,38 +2388,38 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="G44"/>
       <c r="H44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="I44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="J44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="K44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="L44" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="M44" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45">
@@ -2187,7 +2427,7 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C45"/>
       <c r="D45"/>
@@ -2197,13 +2437,13 @@
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="K45" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="L45" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="M45"/>
     </row>
@@ -2212,38 +2452,38 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="G46"/>
       <c r="H46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="I46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="J46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="K46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="L46" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="M46" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47">
@@ -2251,38 +2491,38 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="G47"/>
       <c r="H47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="I47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="J47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="K47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="L47" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M47" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48">
@@ -2290,38 +2530,38 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="F48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G48"/>
       <c r="H48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="I48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="J48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="K48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="L48" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="M48" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>